<commit_message>
Add i.MX8MPPWREVK A1 revision / change eeprom board detection
To detect connected board PMT now checks the BOARD_ID and BOARD_REV stored
in the EEPROM. User should specify board revision in command line for
a board with many revisions (i.e imx8mppwrevka0 or imx8mppwrevka1).
Board supported  with different revisions can be list with lsboard command.

Signed-off-by: Mathis Deroo <mathis.deroo@nxp.com>
</commit_message>
<xml_diff>
--- a/docs/EEPROM_Programmer_Tool.xlsx
+++ b/docs/EEPROM_Programmer_Tool.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="158">
   <si>
     <t xml:space="preserve">Instructions:</t>
   </si>
@@ -178,7 +178,7 @@
     <t xml:space="preserve">0x15</t>
   </si>
   <si>
-    <t xml:space="preserve">NXP i.MX8MP DDR4L Board</t>
+    <t xml:space="preserve">NXP i.MX8MP DDR4 Board</t>
   </si>
   <si>
     <t xml:space="preserve">0x06</t>
@@ -360,9 +360,6 @@
   </si>
   <si>
     <t xml:space="preserve">0x6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NXP i.MX8MP DDR4 Board</t>
   </si>
   <si>
     <t xml:space="preserve">…</t>
@@ -924,7 +921,7 @@
   </sheetPr>
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -998,7 +995,7 @@
   </sheetPr>
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -1006,7 +1003,7 @@
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="2" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="2" width="11.3562753036437"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="32.9919028340081"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="33.2064777327935"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="2" width="8.89068825910931"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="3" width="8.89068825910931"/>
   </cols>
@@ -1225,14 +1222,14 @@
   <dimension ref="A1:W32"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N39" activeCellId="0" sqref="N39"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="32.1376518218623"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="32.3481781376518"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="21.3157894736842"/>
     <col collapsed="false" hidden="false" max="9" min="6" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="11" min="10" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.57085020242915"/>
@@ -1240,7 +1237,7 @@
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="17" min="16" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="20" min="19" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="20" min="19" style="0" width="19.8178137651822"/>
     <col collapsed="false" hidden="false" max="21" min="21" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="22" min="22" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="8.57085020242915"/>
@@ -2167,13 +2164,13 @@
   <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="8" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="18.1012145748988"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="18.2105263157895"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="8" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="8" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="8" width="20.7813765182186"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="8" width="9"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="8" width="32.6720647773279"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="9" width="66.8421052631579"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="8" width="32.8866396761134"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="9" width="67.4858299595142"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="9" width="9"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="9" width="8.89068825910931"/>
   </cols>
@@ -12528,7 +12525,7 @@
         <v>111</v>
       </c>
       <c r="H12" s="22" t="s">
-        <v>112</v>
+        <v>51</v>
       </c>
       <c r="I12" s="25"/>
       <c r="J12" s="0"/>
@@ -13555,10 +13552,10 @@
       <c r="E13" s="23"/>
       <c r="F13" s="24"/>
       <c r="G13" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="H13" s="22" t="s">
         <v>113</v>
-      </c>
-      <c r="H13" s="22" t="s">
-        <v>114</v>
       </c>
       <c r="I13" s="25"/>
       <c r="J13" s="0"/>
@@ -14598,13 +14595,13 @@
         <v>13</v>
       </c>
       <c r="C15" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="D15" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="D15" s="28" t="s">
+      <c r="E15" s="16" t="s">
         <v>116</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>117</v>
       </c>
       <c r="F15" s="29" t="s">
         <v>12</v>
@@ -14613,10 +14610,10 @@
         <v>107</v>
       </c>
       <c r="H15" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="I15" s="30" t="s">
         <v>118</v>
-      </c>
-      <c r="I15" s="30" t="s">
-        <v>119</v>
       </c>
       <c r="J15" s="31"/>
     </row>
@@ -14631,7 +14628,7 @@
         <v>108</v>
       </c>
       <c r="H16" s="22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I16" s="30"/>
       <c r="J16" s="31"/>
@@ -14647,7 +14644,7 @@
         <v>100</v>
       </c>
       <c r="H17" s="22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I17" s="30"/>
       <c r="J17" s="31"/>
@@ -14663,7 +14660,7 @@
         <v>109</v>
       </c>
       <c r="H18" s="22" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I18" s="30"/>
       <c r="J18" s="31"/>
@@ -14672,18 +14669,18 @@
       <c r="A19" s="27"/>
       <c r="B19" s="15"/>
       <c r="C19" s="23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D19" s="28"/>
       <c r="E19" s="23" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F19" s="29"/>
       <c r="G19" s="22" t="s">
         <v>107</v>
       </c>
       <c r="H19" s="22" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I19" s="30"/>
       <c r="J19" s="31"/>
@@ -14699,7 +14696,7 @@
         <v>108</v>
       </c>
       <c r="H20" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I20" s="30"/>
       <c r="J20" s="31"/>
@@ -14715,7 +14712,7 @@
         <v>100</v>
       </c>
       <c r="H21" s="22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I21" s="30"/>
       <c r="J21" s="31"/>
@@ -14731,7 +14728,7 @@
         <v>109</v>
       </c>
       <c r="H22" s="23" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I22" s="30"/>
       <c r="J22" s="31"/>
@@ -14744,10 +14741,10 @@
         <v>16</v>
       </c>
       <c r="C23" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="D23" s="28" t="s">
         <v>129</v>
-      </c>
-      <c r="D23" s="28" t="s">
-        <v>130</v>
       </c>
       <c r="E23" s="28"/>
       <c r="F23" s="29" t="s">
@@ -14760,7 +14757,7 @@
         <v>35</v>
       </c>
       <c r="I23" s="32" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14786,7 +14783,7 @@
       <c r="E25" s="28"/>
       <c r="F25" s="29"/>
       <c r="G25" s="22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H25" s="22"/>
       <c r="I25" s="32"/>
@@ -14854,13 +14851,13 @@
         <v>19</v>
       </c>
       <c r="C31" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="D31" s="28" t="s">
         <v>132</v>
       </c>
-      <c r="D31" s="28" t="s">
-        <v>133</v>
-      </c>
       <c r="E31" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F31" s="29" t="s">
         <v>18</v>
@@ -14869,10 +14866,10 @@
         <v>107</v>
       </c>
       <c r="H31" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="I31" s="30" t="s">
         <v>118</v>
-      </c>
-      <c r="I31" s="30" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14886,7 +14883,7 @@
         <v>108</v>
       </c>
       <c r="H32" s="22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I32" s="30"/>
     </row>
@@ -14901,7 +14898,7 @@
         <v>100</v>
       </c>
       <c r="H33" s="22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I33" s="30"/>
     </row>
@@ -14916,7 +14913,7 @@
         <v>109</v>
       </c>
       <c r="H34" s="22" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I34" s="30"/>
     </row>
@@ -14924,18 +14921,18 @@
       <c r="A35" s="27"/>
       <c r="B35" s="15"/>
       <c r="C35" s="23" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D35" s="28"/>
       <c r="E35" s="23" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F35" s="29"/>
       <c r="G35" s="22" t="s">
         <v>110</v>
       </c>
       <c r="H35" s="22" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I35" s="30"/>
     </row>
@@ -14950,7 +14947,7 @@
         <v>111</v>
       </c>
       <c r="H36" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I36" s="30"/>
     </row>
@@ -14962,10 +14959,10 @@
       <c r="E37" s="23"/>
       <c r="F37" s="29"/>
       <c r="G37" s="22" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H37" s="22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I37" s="30"/>
     </row>
@@ -14977,10 +14974,10 @@
       <c r="E38" s="23"/>
       <c r="F38" s="29"/>
       <c r="G38" s="23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H38" s="23" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I38" s="30"/>
     </row>
@@ -14992,10 +14989,10 @@
         <v>22</v>
       </c>
       <c r="C39" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="D39" s="28" t="s">
         <v>137</v>
-      </c>
-      <c r="D39" s="28" t="s">
-        <v>138</v>
       </c>
       <c r="E39" s="28"/>
       <c r="F39" s="29" t="s">
@@ -15005,10 +15002,10 @@
         <v>107</v>
       </c>
       <c r="H39" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="I39" s="33" t="s">
         <v>139</v>
-      </c>
-      <c r="I39" s="33" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15025,7 +15022,7 @@
         <v>23</v>
       </c>
       <c r="I40" s="34" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15102,13 +15099,13 @@
         <v>25</v>
       </c>
       <c r="C47" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="D47" s="28" t="s">
         <v>142</v>
       </c>
-      <c r="D47" s="28" t="s">
-        <v>143</v>
-      </c>
       <c r="E47" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F47" s="29" t="s">
         <v>24</v>
@@ -15117,10 +15114,10 @@
         <v>107</v>
       </c>
       <c r="H47" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I47" s="35" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15134,7 +15131,7 @@
         <v>108</v>
       </c>
       <c r="H48" s="22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I48" s="35"/>
     </row>
@@ -15146,10 +15143,10 @@
       <c r="E49" s="16"/>
       <c r="F49" s="29"/>
       <c r="G49" s="22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H49" s="22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I49" s="35"/>
     </row>
@@ -15161,10 +15158,10 @@
       <c r="E50" s="16"/>
       <c r="F50" s="29"/>
       <c r="G50" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="H50" s="22" t="s">
         <v>145</v>
-      </c>
-      <c r="H50" s="22" t="s">
-        <v>146</v>
       </c>
       <c r="I50" s="35"/>
     </row>
@@ -15172,18 +15169,18 @@
       <c r="A51" s="27"/>
       <c r="B51" s="15"/>
       <c r="C51" s="23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D51" s="28"/>
       <c r="E51" s="23" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F51" s="29"/>
       <c r="G51" s="22" t="s">
         <v>107</v>
       </c>
       <c r="H51" s="22" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I51" s="35"/>
     </row>
@@ -15198,7 +15195,7 @@
         <v>108</v>
       </c>
       <c r="H52" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I52" s="35"/>
     </row>
@@ -15210,10 +15207,10 @@
       <c r="E53" s="23"/>
       <c r="F53" s="29"/>
       <c r="G53" s="22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H53" s="22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I53" s="35"/>
     </row>
@@ -15225,10 +15222,10 @@
       <c r="E54" s="23"/>
       <c r="F54" s="29"/>
       <c r="G54" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="H54" s="23" t="s">
         <v>145</v>
-      </c>
-      <c r="H54" s="23" t="s">
-        <v>146</v>
       </c>
       <c r="I54" s="35"/>
     </row>
@@ -15240,10 +15237,10 @@
         <v>28</v>
       </c>
       <c r="C55" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="D55" s="28" t="s">
         <v>148</v>
-      </c>
-      <c r="D55" s="28" t="s">
-        <v>149</v>
       </c>
       <c r="E55" s="28"/>
       <c r="F55" s="29" t="s">
@@ -15253,7 +15250,7 @@
         <v>107</v>
       </c>
       <c r="H55" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I55" s="32"/>
     </row>
@@ -15268,7 +15265,7 @@
         <v>108</v>
       </c>
       <c r="H56" s="22" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I56" s="32"/>
     </row>
@@ -15283,7 +15280,7 @@
         <v>100</v>
       </c>
       <c r="H57" s="22" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I57" s="32"/>
     </row>
@@ -15298,7 +15295,7 @@
         <v>109</v>
       </c>
       <c r="H58" s="22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I58" s="32"/>
     </row>
@@ -15310,7 +15307,7 @@
       <c r="E59" s="28"/>
       <c r="F59" s="29"/>
       <c r="G59" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H59" s="22"/>
       <c r="I59" s="32"/>
@@ -15353,13 +15350,13 @@
         <v>2</v>
       </c>
       <c r="B63" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="C63" s="28" t="s">
         <v>155</v>
       </c>
-      <c r="C63" s="28" t="s">
+      <c r="D63" s="28" t="s">
         <v>156</v>
-      </c>
-      <c r="D63" s="28" t="s">
-        <v>157</v>
       </c>
       <c r="E63" s="28"/>
       <c r="F63" s="29" t="s">
@@ -15370,7 +15367,7 @@
       </c>
       <c r="H63" s="16"/>
       <c r="I63" s="36" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15394,7 +15391,7 @@
       <c r="E65" s="28"/>
       <c r="F65" s="29"/>
       <c r="G65" s="22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H65" s="22"/>
       <c r="I65" s="36"/>

</xml_diff>